<commit_message>
fleshed out models with commented logic and some code
</commit_message>
<xml_diff>
--- a/doc/MVC.xlsx
+++ b/doc/MVC.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\pr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\pr\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="19560" windowHeight="8340"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="19560" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="35">
   <si>
     <t>Models</t>
   </si>
@@ -519,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,9 +626,6 @@
       <c r="D3" t="s">
         <v>28</v>
       </c>
-      <c r="E3" t="s">
-        <v>28</v>
-      </c>
       <c r="J3" t="s">
         <v>12</v>
       </c>

</xml_diff>